<commit_message>
Added milk run cost calculations. Turns out, nearest neighbour milk-run with our assumptions performs worse than direct shipping!
</commit_message>
<xml_diff>
--- a/msci_434_supplimental_calculations.xlsx
+++ b/msci_434_supplimental_calculations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinn Turner\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\transportation_supplier_warehouse_store_cplex_heuristic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A735D9E2-6C7E-45E0-861F-F8A6461538C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDB1FF6-C922-4085-81E0-3664EF8619F6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{A48016D2-0034-4139-BC47-AF820BC0AF08}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>1</t>
   </si>
@@ -82,6 +82,54 @@
   </si>
   <si>
     <t>Ordered list of stores closest to each warehouse (smallest --&gt; largest)</t>
+  </si>
+  <si>
+    <t>Warehouse to store distances</t>
+  </si>
+  <si>
+    <t>Store to store distance</t>
+  </si>
+  <si>
+    <t>Store locations</t>
+  </si>
+  <si>
+    <t>Warehouse locations</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Cost ($) to travel from warehouse&lt;--&gt;store</t>
   </si>
 </sst>
 </file>
@@ -287,10 +335,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D8353433-FD27-4D16-B1EA-F8C83CE39D9A}" name="Table8" displayName="Table8" ref="I1:S11" totalsRowShown="0">
-  <autoFilter ref="I1:S11" xr:uid="{FBA53A29-8CFC-485E-BA48-51B845674135}"/>
-  <sortState ref="I2:S11">
-    <sortCondition ref="I1:I11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D8353433-FD27-4D16-B1EA-F8C83CE39D9A}" name="Table8" displayName="Table8" ref="M2:W12" totalsRowShown="0">
+  <autoFilter ref="M2:W12" xr:uid="{FBA53A29-8CFC-485E-BA48-51B845674135}"/>
+  <sortState ref="M3:W12">
+    <sortCondition ref="M2:M12"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{FFDAF3F9-A0AA-4F2D-AC03-9E86F2356C7C}" name="Store"/>
@@ -310,10 +358,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{84A435BB-992D-4FCF-84F1-14569D05AF61}" name="Table13" displayName="Table13" ref="M14:N24" totalsRowShown="0">
-  <autoFilter ref="M14:N24" xr:uid="{4B2173B5-772C-42CF-8B63-E750BD920CA8}"/>
-  <sortState ref="M15:N24">
-    <sortCondition ref="N14:N24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{84A435BB-992D-4FCF-84F1-14569D05AF61}" name="Table13" displayName="Table13" ref="M15:N25" totalsRowShown="0">
+  <autoFilter ref="M15:N25" xr:uid="{4B2173B5-772C-42CF-8B63-E750BD920CA8}"/>
+  <sortState ref="M16:N25">
+    <sortCondition ref="N15:N25"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{21D4F6C1-3EB6-4655-B1B1-A3CDA3F7CEAF}" name="Store"/>
@@ -324,10 +372,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E9DFC1BE-173F-4589-9708-8E09546B5B4E}" name="Table14" displayName="Table14" ref="P14:Q24" totalsRowShown="0">
-  <autoFilter ref="P14:Q24" xr:uid="{C82FD9A7-1A09-4B41-9366-3A4F314793EE}"/>
-  <sortState ref="P15:Q24">
-    <sortCondition ref="Q14:Q24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E9DFC1BE-173F-4589-9708-8E09546B5B4E}" name="Table14" displayName="Table14" ref="P15:Q25" totalsRowShown="0">
+  <autoFilter ref="P15:Q25" xr:uid="{C82FD9A7-1A09-4B41-9366-3A4F314793EE}"/>
+  <sortState ref="P16:Q25">
+    <sortCondition ref="Q15:Q25"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8452F432-F81F-49FB-8B03-8969A777FC99}" name="Store"/>
@@ -338,8 +386,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{90B9DC4B-B6C8-43E7-AAA8-6E8CB5057398}" name="Table15" displayName="Table15" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{9000613B-B622-4827-95B9-A2E7236B8453}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{90B9DC4B-B6C8-43E7-AAA8-6E8CB5057398}" name="Table15" displayName="Table15" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4" xr:uid="{9000613B-B622-4827-95B9-A2E7236B8453}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{233D9924-12BA-4D9C-9A38-AB57136656FF}" name="Warehouse"/>
     <tableColumn id="2" xr3:uid="{4E632CB8-6698-45B3-A465-DEF23764954B}" name="X"/>
@@ -350,12 +398,28 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C0AFE834-0267-467D-8F5D-0B917CB7767A}" name="Table16" displayName="Table16" ref="E1:G11" totalsRowShown="0">
-  <autoFilter ref="E1:G11" xr:uid="{93D5D7A6-7614-4812-BCEC-AFAFBDE727F0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C0AFE834-0267-467D-8F5D-0B917CB7767A}" name="Table16" displayName="Table16" ref="E2:G12" totalsRowShown="0">
+  <autoFilter ref="E2:G12" xr:uid="{93D5D7A6-7614-4812-BCEC-AFAFBDE727F0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8F375813-E6D0-4E82-9E4D-023936503CF6}" name="Store"/>
     <tableColumn id="2" xr3:uid="{715FD534-DFB7-4808-8AA5-AE1FF2B1BA5F}" name="X" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{CE860815-B0AB-40D6-96F0-3A762B0D61C2}" name="Y" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA95427C-9861-4B68-8B49-3A4CF0FED205}" name="Table1" displayName="Table1" ref="I2:K12" totalsRowShown="0">
+  <autoFilter ref="I2:K12" xr:uid="{DF8016F5-A68E-451D-8D16-1CCA91C4E4DA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AEDA76DE-5F98-46DE-BE89-091CF2C80FC5}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{A3298EE0-DFDD-4318-BE36-A29B8F90B6D6}" name="W1">
+      <calculatedColumnFormula>SQRT((F3-$B$3)^2+(G3-$C$3)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{3D0DD08D-41A9-4687-BF3B-987090AA7ADA}" name="W2">
+      <calculatedColumnFormula>SQRT((F3-$B$4)^2+(G3-$C$4)^2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96A46C9-C1E4-426B-A67C-AE99D3DA06DE}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,618 +737,707 @@
     <col min="11" max="16" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N2" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R2" t="s">
         <v>4</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V2" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>27</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>23</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <v>38</v>
       </c>
-      <c r="I2">
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3">
+        <f>SQRT((F3-$B$3)^2+(G3-$C$3)^2)</f>
+        <v>17.029386365926403</v>
+      </c>
+      <c r="K3">
+        <f>SQRT((F3-$B$4)^2+(G3-$C$4)^2)</f>
+        <v>274.04561664073373</v>
+      </c>
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="N3">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="O3">
         <v>113.52973178863765</v>
       </c>
-      <c r="L2">
+      <c r="P3">
         <v>282.79321066814884</v>
       </c>
-      <c r="M2">
+      <c r="Q3">
         <v>202.20039564748632</v>
       </c>
-      <c r="N2">
+      <c r="R3">
         <v>183.41210428976601</v>
       </c>
-      <c r="O2">
+      <c r="S3">
         <v>330.80054413498175</v>
       </c>
-      <c r="P2">
+      <c r="T3">
         <v>110.45361017187261</v>
       </c>
-      <c r="Q2">
+      <c r="U3">
         <v>236.68544526438461</v>
       </c>
-      <c r="R2">
+      <c r="V3">
         <v>128.31601614763451</v>
       </c>
-      <c r="S2">
+      <c r="W3">
         <v>175.96022277776305</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>253</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>187</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <v>58</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="2">
         <v>146</v>
       </c>
-      <c r="I3">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <f>SQRT((F4-$B$3)^2+(G4-$C$3)^2)</f>
+        <v>128.31601614763451</v>
+      </c>
+      <c r="K4">
+        <f>SQRT((F4-$B$4)^2+(G4-$C$4)^2)</f>
+        <v>199.26364445126461</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="N4">
         <v>113.52973178863765</v>
       </c>
-      <c r="K3">
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="L3">
+      <c r="P4">
         <v>231.31147831441481</v>
       </c>
-      <c r="M3">
+      <c r="Q4">
         <v>186.95453992882869</v>
       </c>
-      <c r="N3">
+      <c r="R4">
         <v>128.89142717807107</v>
       </c>
-      <c r="O3">
+      <c r="S4">
         <v>268.36169622358551</v>
       </c>
-      <c r="P3">
+      <c r="T4">
         <v>58.008620049092706</v>
       </c>
-      <c r="Q3">
+      <c r="U4">
         <v>139.78912690191609</v>
       </c>
-      <c r="R3">
+      <c r="V4">
         <v>166.73931749890306</v>
       </c>
-      <c r="S3">
+      <c r="W4">
         <v>62.585940913275401</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E4" s="1">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>289</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="2">
         <v>134</v>
       </c>
-      <c r="I4">
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5">
+        <f>SQRT((F5-$B$3)^2+(G5-$C$3)^2)</f>
+        <v>298.81432361920002</v>
+      </c>
+      <c r="K5">
+        <f>SQRT((F5-$B$4)^2+(G5-$C$4)^2)</f>
+        <v>64.070273918565391</v>
+      </c>
+      <c r="M5">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="N5">
         <v>282.79321066814884</v>
       </c>
-      <c r="K4">
+      <c r="O5">
         <v>231.31147831441481</v>
       </c>
-      <c r="L4">
+      <c r="P5">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="Q5">
         <v>98.493654617949886</v>
       </c>
-      <c r="N4">
+      <c r="R5">
         <v>104.47966309287182</v>
       </c>
-      <c r="O4">
+      <c r="S5">
         <v>53.075418038862395</v>
       </c>
-      <c r="P4">
+      <c r="T5">
         <v>185.31055015837603</v>
       </c>
-      <c r="Q4">
+      <c r="U5">
         <v>137.20058308913997</v>
       </c>
-      <c r="R4">
+      <c r="V5">
         <v>191.84629264074925</v>
       </c>
-      <c r="S4">
+      <c r="W5">
         <v>228.94977615188881</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E5" s="1">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E6" s="1">
         <v>4</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>224</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G6" s="2">
         <v>60</v>
       </c>
-      <c r="I5">
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <f>SQRT((F6-$B$3)^2+(G6-$C$3)^2)</f>
+        <v>216.52944372532804</v>
+      </c>
+      <c r="K6">
+        <f>SQRT((F6-$B$4)^2+(G6-$C$4)^2)</f>
+        <v>130.26895255585654</v>
+      </c>
+      <c r="M6">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="N6">
         <v>202.20039564748632</v>
       </c>
-      <c r="K5">
+      <c r="O6">
         <v>186.95453992882869</v>
       </c>
-      <c r="L5">
+      <c r="P6">
         <v>98.493654617949886</v>
       </c>
-      <c r="M5">
+      <c r="Q6">
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="R6">
         <v>74.94664769020693</v>
       </c>
-      <c r="O5">
+      <c r="S6">
         <v>151.55856953666461</v>
       </c>
-      <c r="P5">
+      <c r="T6">
         <v>129.86531484580476</v>
       </c>
-      <c r="Q5">
+      <c r="U6">
         <v>162.36070953281771</v>
       </c>
-      <c r="R5">
+      <c r="V6">
         <v>94.62557793746889</v>
       </c>
-      <c r="S5">
+      <c r="W6">
         <v>211.45448682872635</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E6" s="1">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E7" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>185</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G7" s="2">
         <v>124</v>
       </c>
-      <c r="I6">
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <f>SQRT((F7-$B$3)^2+(G7-$C$3)^2)</f>
+        <v>200.08498194517247</v>
+      </c>
+      <c r="K7">
+        <f>SQRT((F7-$B$4)^2+(G7-$C$4)^2)</f>
+        <v>92.69843580125827</v>
+      </c>
+      <c r="M7">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="N7">
         <v>183.41210428976601</v>
       </c>
-      <c r="K6">
+      <c r="O7">
         <v>128.89142717807107</v>
       </c>
-      <c r="L6">
+      <c r="P7">
         <v>104.47966309287182</v>
       </c>
-      <c r="M6">
+      <c r="Q7">
         <v>74.94664769020693</v>
       </c>
-      <c r="N6">
+      <c r="R7">
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="S7">
         <v>148.32734070291963</v>
       </c>
-      <c r="P6">
+      <c r="T7">
         <v>80.894993664626739</v>
       </c>
-      <c r="Q6">
+      <c r="U7">
         <v>92.195444572928878</v>
       </c>
-      <c r="R6">
+      <c r="V7">
         <v>124.91997438360288</v>
       </c>
-      <c r="S6">
+      <c r="W7">
         <v>140.20698984002189</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E7" s="1">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E8" s="1">
         <v>6</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>325</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>173</v>
       </c>
-      <c r="I7">
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8">
+        <f>SQRT((F8-$B$3)^2+(G8-$C$3)^2)</f>
+        <v>347.19014962985341</v>
+      </c>
+      <c r="K8">
+        <f>SQRT((F8-$B$4)^2+(G8-$C$4)^2)</f>
+        <v>73.348483283568996</v>
+      </c>
+      <c r="M8">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="N8">
         <v>330.80054413498175</v>
       </c>
-      <c r="K7">
+      <c r="O8">
         <v>268.36169622358551</v>
       </c>
-      <c r="L7">
+      <c r="P8">
         <v>53.075418038862395</v>
       </c>
-      <c r="M7">
+      <c r="Q8">
         <v>151.55856953666461</v>
       </c>
-      <c r="N7">
+      <c r="R8">
         <v>148.32734070291963</v>
       </c>
-      <c r="O7">
+      <c r="S8">
         <v>0</v>
       </c>
-      <c r="P7">
+      <c r="T8">
         <v>228.30024091095481</v>
       </c>
-      <c r="Q7">
+      <c r="U8">
         <v>152.20052562327109</v>
       </c>
-      <c r="R7">
+      <c r="V8">
         <v>244.76110802167898</v>
       </c>
-      <c r="S7">
+      <c r="W8">
         <v>255.27436220662662</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E8" s="1">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E9" s="1">
         <v>7</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>105</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>112</v>
       </c>
-      <c r="I8">
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9">
+        <f>SQRT((F9-$B$3)^2+(G9-$C$3)^2)</f>
+        <v>127.47548783981962</v>
+      </c>
+      <c r="K9">
+        <f>SQRT((F9-$B$4)^2+(G9-$C$4)^2)</f>
+        <v>165.91865476793137</v>
+      </c>
+      <c r="M9">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="N9">
         <v>110.45361017187261</v>
       </c>
-      <c r="K8">
+      <c r="O9">
         <v>58.008620049092706</v>
       </c>
-      <c r="L8">
+      <c r="P9">
         <v>185.31055015837603</v>
       </c>
-      <c r="M8">
+      <c r="Q9">
         <v>129.86531484580476</v>
       </c>
-      <c r="N8">
+      <c r="R9">
         <v>80.894993664626739</v>
       </c>
-      <c r="O8">
+      <c r="S9">
         <v>228.30024091095481</v>
       </c>
-      <c r="P8">
+      <c r="T9">
         <v>0</v>
       </c>
-      <c r="Q8">
+      <c r="U9">
         <v>127.6401190848708</v>
       </c>
-      <c r="R8">
+      <c r="V9">
         <v>114.94781424629178</v>
       </c>
-      <c r="S8">
+      <c r="W9">
         <v>100.56838469419701</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E9" s="1">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E10" s="1">
         <v>8</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>179</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>216</v>
       </c>
-      <c r="I9">
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10">
+        <f>SQRT((F10-$B$3)^2+(G10-$C$3)^2)</f>
+        <v>253.53895164254348</v>
+      </c>
+      <c r="K10">
+        <f>SQRT((F10-$B$4)^2+(G10-$C$4)^2)</f>
+        <v>79.479557120054466</v>
+      </c>
+      <c r="M10">
         <v>8</v>
       </c>
-      <c r="J9">
+      <c r="N10">
         <v>236.68544526438461</v>
       </c>
-      <c r="K9">
+      <c r="O10">
         <v>139.78912690191609</v>
       </c>
-      <c r="L9">
+      <c r="P10">
         <v>137.20058308913997</v>
       </c>
-      <c r="M9">
+      <c r="Q10">
         <v>162.36070953281771</v>
       </c>
-      <c r="N9">
+      <c r="R10">
         <v>92.195444572928878</v>
       </c>
-      <c r="O9">
+      <c r="S10">
         <v>152.20052562327109</v>
       </c>
-      <c r="P9">
+      <c r="T10">
         <v>127.6401190848708</v>
       </c>
-      <c r="Q9">
+      <c r="U10">
         <v>0</v>
       </c>
-      <c r="R9">
+      <c r="V10">
         <v>213.41274563624359</v>
       </c>
-      <c r="S9">
+      <c r="W10">
         <v>107.37783756436893</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E10" s="1">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E11" s="1">
         <v>9</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>147</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="I10">
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11">
+        <f>SQRT((F11-$B$3)^2+(G11-$C$3)^2)</f>
+        <v>138.75518008348374</v>
+      </c>
+      <c r="K11">
+        <f>SQRT((F11-$B$4)^2+(G11-$C$4)^2)</f>
+        <v>210.61813787041228</v>
+      </c>
+      <c r="M11">
         <v>9</v>
       </c>
-      <c r="J10">
+      <c r="N11">
         <v>128.31601614763451</v>
       </c>
-      <c r="K10">
+      <c r="O11">
         <v>166.73931749890306</v>
       </c>
-      <c r="L10">
+      <c r="P11">
         <v>191.84629264074925</v>
       </c>
-      <c r="M10">
+      <c r="Q11">
         <v>94.62557793746889</v>
       </c>
-      <c r="N10">
+      <c r="R11">
         <v>124.91997438360288</v>
       </c>
-      <c r="O10">
+      <c r="S11">
         <v>244.76110802167898</v>
       </c>
-      <c r="P10">
+      <c r="T11">
         <v>114.94781424629178</v>
       </c>
-      <c r="Q10">
+      <c r="U11">
         <v>213.41274563624359</v>
       </c>
-      <c r="R10">
+      <c r="V11">
         <v>0</v>
       </c>
-      <c r="S10">
+      <c r="W11">
         <v>215.4738963308549</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E11" s="1">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E12" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>72</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>207</v>
       </c>
-      <c r="I11">
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12">
+        <f>SQRT((F12-$B$3)^2+(G12-$C$3)^2)</f>
+        <v>190.37857022259621</v>
+      </c>
+      <c r="K12">
+        <f>SQRT((F12-$B$4)^2+(G12-$C$4)^2)</f>
+        <v>182.10161998181127</v>
+      </c>
+      <c r="M12">
         <v>10</v>
       </c>
-      <c r="J11">
+      <c r="N12">
         <v>175.96022277776305</v>
       </c>
-      <c r="K11">
+      <c r="O12">
         <v>62.585940913275401</v>
       </c>
-      <c r="L11">
+      <c r="P12">
         <v>228.94977615188881</v>
       </c>
-      <c r="M11">
+      <c r="Q12">
         <v>211.45448682872635</v>
       </c>
-      <c r="N11">
+      <c r="R12">
         <v>140.20698984002189</v>
       </c>
-      <c r="O11">
+      <c r="S12">
         <v>255.27436220662662</v>
       </c>
-      <c r="P11">
+      <c r="T12">
         <v>100.56838469419701</v>
       </c>
-      <c r="Q11">
+      <c r="U12">
         <v>107.37783756436893</v>
       </c>
-      <c r="R11">
+      <c r="V12">
         <v>215.4738963308549</v>
       </c>
-      <c r="S11">
+      <c r="W12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M13" t="s">
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
-      <c r="M14" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="M15" t="s">
         <v>16</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N15" t="s">
         <v>10</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P15" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
         <v>1</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
-        <v>5</v>
-      </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
-      <c r="H15" s="1">
-        <v>8</v>
-      </c>
-      <c r="I15" s="1">
-        <v>3</v>
-      </c>
-      <c r="J15" s="3">
-        <v>6</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>28.284271247461902</v>
-      </c>
-      <c r="P15">
-        <v>8</v>
-      </c>
-      <c r="Q15">
-        <v>37.8549864614954</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>2</v>
       </c>
       <c r="B16" s="1">
         <v>7</v>
       </c>
       <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1">
         <v>10</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>5</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
         <v>8</v>
-      </c>
-      <c r="G16" s="1">
-        <v>9</v>
-      </c>
-      <c r="H16" s="1">
-        <v>4</v>
       </c>
       <c r="I16" s="1">
         <v>3</v>
@@ -1293,379 +1446,531 @@
         <v>6</v>
       </c>
       <c r="M16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N16">
-        <v>120.10412149464314</v>
+        <v>28.284271247461902</v>
       </c>
       <c r="P16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q16">
-        <v>123.8587905640936</v>
+        <v>37.8549864614954</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>8</v>
-      </c>
-      <c r="F17" s="1">
-        <v>7</v>
       </c>
       <c r="G17" s="1">
         <v>9</v>
       </c>
       <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>6</v>
+      </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
+      <c r="N17">
+        <v>120.10412149464314</v>
+      </c>
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="I17" s="1">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>7</v>
-      </c>
-      <c r="N17">
-        <v>128.40560735419618</v>
-      </c>
-      <c r="P17">
-        <v>5</v>
-      </c>
       <c r="Q17">
-        <v>129.01550294441361</v>
+        <v>123.8587905640936</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
         <v>4</v>
       </c>
-      <c r="B18" s="1">
+      <c r="D18" s="1">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="E18" s="1">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1">
         <v>9</v>
       </c>
-      <c r="D18" s="1">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="H18" s="1">
+        <v>10</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <v>7</v>
       </c>
-      <c r="F18" s="1">
-        <v>6</v>
-      </c>
-      <c r="G18" s="1">
-        <v>8</v>
-      </c>
-      <c r="H18" s="1">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
-        <v>10</v>
-      </c>
-      <c r="M18">
-        <v>2</v>
-      </c>
       <c r="N18">
-        <v>139.48835076808385</v>
+        <v>128.40560735419618</v>
       </c>
       <c r="P18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q18">
-        <v>156.73225577397909</v>
+        <v>129.01550294441361</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
         <v>5</v>
       </c>
-      <c r="B19" s="1">
-        <v>4</v>
-      </c>
       <c r="C19" s="1">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
         <v>7</v>
       </c>
-      <c r="D19" s="1">
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1">
         <v>8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>10</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>139.48835076808385</v>
+      </c>
+      <c r="P19">
         <v>3</v>
       </c>
-      <c r="F19" s="1">
-        <v>9</v>
-      </c>
-      <c r="G19" s="1">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1">
-        <v>10</v>
-      </c>
-      <c r="I19" s="1">
-        <v>6</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>5</v>
-      </c>
-      <c r="N19">
-        <v>194.83326204732086</v>
-      </c>
-      <c r="P19">
-        <v>6</v>
-      </c>
       <c r="Q19">
-        <v>159.51175505272332</v>
+        <v>156.73225577397909</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="1">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1">
-        <v>8</v>
-      </c>
       <c r="F20" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G20" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1">
         <v>10</v>
       </c>
       <c r="I20" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J20" s="3">
         <v>1</v>
       </c>
       <c r="M20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N20">
-        <v>202.07424378183381</v>
+        <v>194.83326204732086</v>
       </c>
       <c r="P20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q20">
-        <v>163.11039206623224</v>
+        <v>159.51175505272332</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
       </c>
       <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7</v>
+      </c>
+      <c r="G21" s="1">
+        <v>9</v>
+      </c>
+      <c r="H21" s="1">
         <v>10</v>
       </c>
-      <c r="E21" s="1">
+      <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="1">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1">
-        <v>4</v>
-      </c>
-      <c r="I21" s="1">
-        <v>3</v>
-      </c>
-      <c r="J21" s="3">
-        <v>6</v>
-      </c>
       <c r="M21">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N21">
-        <v>203.24615617521528</v>
+        <v>202.07424378183381</v>
       </c>
       <c r="P21">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q21">
-        <v>167.60071598892409</v>
+        <v>163.11039206623224</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1">
         <v>8</v>
-      </c>
-      <c r="B22" s="1">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1">
-        <v>7</v>
-      </c>
-      <c r="E22" s="1">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>6</v>
       </c>
       <c r="H22" s="1">
         <v>4</v>
       </c>
       <c r="I22" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M22">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N22">
-        <v>256.00781238079435</v>
+        <v>203.24615617521528</v>
       </c>
       <c r="P22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q22">
-        <v>196.51463049859672</v>
+        <v>167.60071598892409</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1">
         <v>7</v>
       </c>
-      <c r="D23" s="1">
-        <v>5</v>
-      </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
       </c>
       <c r="G23" s="1">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1">
+        <v>4</v>
+      </c>
+      <c r="I23" s="1">
+        <v>9</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>8</v>
+      </c>
+      <c r="N23">
+        <v>256.00781238079435</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>196.51463049859672</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
         <v>3</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H24" s="1">
         <v>8</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I24" s="1">
         <v>10</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J24" s="3">
         <v>6</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>3</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>289.86203614823381</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>9</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>251.20509548972132</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="7">
+    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="7">
         <v>10</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C25" s="4">
         <v>7</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D25" s="4">
         <v>8</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E25" s="4">
         <v>5</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F25" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G25" s="4">
         <v>4</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H25" s="4">
         <v>9</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I25" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J25" s="5">
         <v>6</v>
       </c>
-      <c r="M24">
+      <c r="M25">
         <v>6</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <v>339.66601242985735</v>
       </c>
-      <c r="P24">
+      <c r="P25">
         <v>1</v>
       </c>
-      <c r="Q24">
+      <c r="Q25">
         <v>270.40894955603818</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>170.29386365926402</v>
+      </c>
+      <c r="C29">
+        <v>1283.1601614763451</v>
+      </c>
+      <c r="D29">
+        <v>2988.1432361920001</v>
+      </c>
+      <c r="E29">
+        <v>2165.2944372532802</v>
+      </c>
+      <c r="F29">
+        <v>2000.8498194517247</v>
+      </c>
+      <c r="G29">
+        <v>3471.9014962985339</v>
+      </c>
+      <c r="H29">
+        <v>1274.7548783981963</v>
+      </c>
+      <c r="I29">
+        <v>2535.389516425435</v>
+      </c>
+      <c r="J29">
+        <v>1387.5518008348374</v>
+      </c>
+      <c r="K29">
+        <v>1903.785702225962</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>2740.4561664073372</v>
+      </c>
+      <c r="C30">
+        <v>1992.636444512646</v>
+      </c>
+      <c r="D30">
+        <v>640.70273918565385</v>
+      </c>
+      <c r="E30">
+        <v>1302.6895255585655</v>
+      </c>
+      <c r="F30">
+        <v>926.98435801258267</v>
+      </c>
+      <c r="G30">
+        <v>733.48483283568999</v>
+      </c>
+      <c r="H30">
+        <v>1659.1865476793137</v>
+      </c>
+      <c r="I30">
+        <v>794.7955712005446</v>
+      </c>
+      <c r="J30">
+        <v>2106.1813787041228</v>
+      </c>
+      <c r="K30">
+        <v>1821.0161998181127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>